<commit_message>
reworked rates with under writer :-)
</commit_message>
<xml_diff>
--- a/health/premium_tables.xlsx
+++ b/health/premium_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\github.com\kubesure\premium\health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8494B0C-5193-4C3D-8E84-A8E966690747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AB9C96-2208-4605-A94B-D6FBC0086B93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="1" r:id="rId1"/>
@@ -35,25 +35,25 @@
     <t>1A</t>
   </si>
   <si>
-    <t>18-35</t>
-  </si>
-  <si>
-    <t>36-45</t>
-  </si>
-  <si>
-    <t>46-55</t>
-  </si>
-  <si>
-    <t>56-60</t>
-  </si>
-  <si>
-    <t>61-65</t>
-  </si>
-  <si>
-    <t>66-70</t>
-  </si>
-  <si>
-    <t>70above</t>
+    <t>18-30</t>
+  </si>
+  <si>
+    <t>31-44</t>
+  </si>
+  <si>
+    <t>45-56</t>
+  </si>
+  <si>
+    <t>56-61</t>
+  </si>
+  <si>
+    <t>62-66</t>
+  </si>
+  <si>
+    <t>67-75</t>
+  </si>
+  <si>
+    <t>75above</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D36"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <v>1300</v>
+        <v>250</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>2200</v>
+        <v>500</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>2600</v>
+        <v>750</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -561,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>4100</v>
+        <v>950</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -578,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>5900</v>
+        <v>1000</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>7900</v>
+        <v>1100</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -612,7 +612,7 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>10400</v>
+        <v>12000</v>
       </c>
       <c r="E7">
         <v>7</v>

</xml_diff>